<commit_message>
switched to web app
</commit_message>
<xml_diff>
--- a/residence_allocation_data.xlsx
+++ b/residence_allocation_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tinnguyen\Documents\Code\Projects\residence-allocator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B55DF9-4763-4114-998E-BFA02D6284D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{722523A2-772A-4D1C-9D26-E240A8E6F0BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11040" xr2:uid="{1558DEF6-6C37-4150-9CCF-8C8D530D7643}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11040" activeTab="1" xr2:uid="{1558DEF6-6C37-4150-9CCF-8C8D530D7643}"/>
   </bookViews>
   <sheets>
     <sheet name="capacity_female" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="101">
   <si>
     <t>student</t>
   </si>
@@ -45,33 +45,12 @@
     <t>residence</t>
   </si>
   <si>
-    <t>fore</t>
-  </si>
-  <si>
-    <t>oo</t>
-  </si>
-  <si>
-    <t>pala</t>
-  </si>
-  <si>
-    <t>shol</t>
-  </si>
-  <si>
-    <t>purn</t>
-  </si>
-  <si>
-    <t>lucc</t>
-  </si>
-  <si>
     <t>secondi</t>
   </si>
   <si>
     <t>primi</t>
   </si>
   <si>
-    <t>ples</t>
-  </si>
-  <si>
     <t>Female1</t>
   </si>
   <si>
@@ -343,6 +322,24 @@
   </si>
   <si>
     <t>Male35</t>
+  </si>
+  <si>
+    <t>OO</t>
+  </si>
+  <si>
+    <t>FORE</t>
+  </si>
+  <si>
+    <t>PALA</t>
+  </si>
+  <si>
+    <t>LUCC</t>
+  </si>
+  <si>
+    <t>SHOL</t>
+  </si>
+  <si>
+    <t>PLES</t>
   </si>
 </sst>
 </file>
@@ -454,25 +451,25 @@
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>oo</c:v>
+                  <c:v>OO</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>fore</c:v>
+                  <c:v>FORE</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>pala</c:v>
+                  <c:v>PALA</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>purn</c:v>
+                  <c:v>PALA</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>lucc</c:v>
+                  <c:v>LUCC</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>shol</c:v>
+                  <c:v>SHOL</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>ples</c:v>
+                  <c:v>PLES</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -543,25 +540,25 @@
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>oo</c:v>
+                  <c:v>OO</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>fore</c:v>
+                  <c:v>FORE</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>pala</c:v>
+                  <c:v>PALA</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>purn</c:v>
+                  <c:v>PALA</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>lucc</c:v>
+                  <c:v>LUCC</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>shol</c:v>
+                  <c:v>SHOL</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>ples</c:v>
+                  <c:v>PLES</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -856,19 +853,19 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>oo</c:v>
+                  <c:v>OO</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>fore</c:v>
+                  <c:v>FORE</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>pala</c:v>
+                  <c:v>PALA</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>purn</c:v>
+                  <c:v>PALA</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>lucc</c:v>
+                  <c:v>LUCC</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -933,19 +930,19 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>oo</c:v>
+                  <c:v>OO</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>fore</c:v>
+                  <c:v>FORE</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>pala</c:v>
+                  <c:v>PALA</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>purn</c:v>
+                  <c:v>PALA</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>lucc</c:v>
+                  <c:v>LUCC</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2654,7 +2651,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{932AD7BC-7322-48CC-B1D8-642C08DDB1CE}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -2669,10 +2666,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2680,7 +2677,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="C2">
         <v>3</v>
@@ -2694,7 +2691,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="C3">
         <v>8</v>
@@ -2708,7 +2705,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="C4">
         <v>12</v>
@@ -2722,7 +2719,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="C5">
         <v>7</v>
@@ -2736,7 +2733,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="C6">
         <v>10</v>
@@ -2750,7 +2747,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="C7">
         <v>8</v>
@@ -2764,7 +2761,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="C8">
         <v>8</v>
@@ -2783,7 +2780,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3204C5DE-3E4F-4378-BEC8-666180AB1FEA}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
@@ -2798,10 +2795,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2809,7 +2806,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="C2">
         <v>3</v>
@@ -2823,7 +2820,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="C3">
         <v>13</v>
@@ -2837,7 +2834,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="C4">
         <v>10</v>
@@ -2851,7 +2848,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="C5">
         <v>6</v>
@@ -2865,7 +2862,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -2924,28 +2921,28 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E2" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="F2" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="G2" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="H2" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="I2" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -2953,28 +2950,28 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D3" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="E3" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="F3" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="G3" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="H3" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="I3" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -2982,28 +2979,28 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D4" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E4" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="F4" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="G4" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="H4" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="I4" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -3011,28 +3008,28 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D5" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="E5" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="F5" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="G5" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="H5" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="I5" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -3040,28 +3037,28 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D6" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E6" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="F6" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="G6" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="H6" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="I6" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -3069,28 +3066,28 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D7" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E7" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="F7" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="G7" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="H7" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="I7" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -3098,28 +3095,28 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="D8" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E8" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="F8" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="G8" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="H8" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="I8" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -3127,28 +3124,28 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="D9" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E9" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="F9" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="G9" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="H9" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="I9" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -3156,28 +3153,28 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="D10" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E10" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="F10" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="G10" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="H10" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="I10" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -3185,28 +3182,28 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="E11" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="F11" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="G11" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="H11" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="I11" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -3214,28 +3211,28 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="D12" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E12" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="F12" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="G12" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="H12" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="I12" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -3243,28 +3240,28 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="D13" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="E13" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="F13" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="G13" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="H13" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="I13" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -3272,28 +3269,28 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="D14" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="E14" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="F14" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="G14" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="H14" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="I14" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -3301,28 +3298,28 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D15" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="E15" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="F15" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="G15" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="H15" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="I15" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -3330,28 +3327,28 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C16" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D16" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E16" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="F16" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="G16" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="H16" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="I16" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -3359,28 +3356,28 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C17" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="D17" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="E17" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="F17" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="G17" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="H17" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="I17" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -3388,28 +3385,28 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C18" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="D18" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E18" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="F18" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="G18" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="H18" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="I18" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -3417,28 +3414,28 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C19" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D19" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="E19" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="F19" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="G19" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="H19" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="I19" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -3446,28 +3443,28 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C20" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D20" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="E20" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="F20" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="G20" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="H20" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="I20" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -3475,28 +3472,28 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C21" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D21" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E21" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="F21" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="G21" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="H21" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="I21" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -3504,28 +3501,28 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C22" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D22" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E22" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="F22" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="G22" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="H22" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="I22" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -3533,28 +3530,28 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C23" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D23" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E23" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="F23" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="G23" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="H23" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="I23" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -3562,28 +3559,28 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C24" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D24" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E24" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="F24" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="G24" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="H24" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="I24" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -3591,28 +3588,28 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C25" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D25" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E25" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="F25" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="G25" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="H25" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="I25" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -3620,28 +3617,28 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C26" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D26" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E26" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="F26" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="G26" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="H26" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="I26" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -3649,28 +3646,28 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C27" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D27" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E27" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="F27" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="G27" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="H27" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="I27" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -3678,28 +3675,28 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C28" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D28" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E28" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="F28" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="G28" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="H28" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="I28" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -3707,28 +3704,28 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C29" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D29" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E29" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="F29" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="G29" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="H29" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="I29" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -3736,28 +3733,28 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C30" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D30" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="E30" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="F30" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="G30" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="H30" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="I30" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -3765,28 +3762,28 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C31" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D31" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E31" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="F31" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="G31" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="H31" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="I31" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -3794,28 +3791,28 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C32" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D32" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E32" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="F32" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="G32" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="H32" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="I32" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -3823,28 +3820,28 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C33" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D33" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E33" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="F33" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="G33" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="H33" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="I33" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -3852,28 +3849,28 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C34" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D34" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E34" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="F34" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="G34" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="H34" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="I34" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -3881,28 +3878,28 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C35" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D35" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E35" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="F35" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="G35" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="H35" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="I35" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -3910,28 +3907,28 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C36" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D36" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E36" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="F36" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="G36" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="H36" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="I36" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -3939,28 +3936,28 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C37" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D37" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E37" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="F37" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="G37" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="H37" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="I37" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -3968,28 +3965,28 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C38" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D38" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E38" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="F38" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="G38" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="H38" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="I38" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -3997,28 +3994,28 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C39" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D39" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="E39" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="F39" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="G39" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="H39" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="I39" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -4026,28 +4023,28 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C40" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D40" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E40" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="F40" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="G40" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="H40" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="I40" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -4055,28 +4052,28 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C41" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="D41" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="E41" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="F41" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="G41" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="H41" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="I41" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -4084,28 +4081,28 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C42" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D42" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E42" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="F42" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="G42" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="H42" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="I42" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -4113,28 +4110,28 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C43" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="D43" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E43" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="F43" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="G43" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="H43" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="I43" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -4142,28 +4139,28 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C44" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="D44" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E44" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="F44" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="G44" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="H44" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="I44" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -4171,28 +4168,28 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C45" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="D45" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E45" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="F45" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="G45" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="H45" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="I45" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -4200,28 +4197,28 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C46" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="D46" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="E46" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="F46" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="G46" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="H46" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="I46" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -4229,28 +4226,28 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C47" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="D47" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="E47" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="F47" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="G47" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="H47" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="I47" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -4258,28 +4255,28 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C48" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="D48" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E48" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="F48" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="G48" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="H48" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="I48" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -4287,28 +4284,28 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C49" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="D49" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E49" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="F49" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="G49" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="H49" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="I49" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
@@ -4316,28 +4313,28 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C50" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="D50" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E50" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="F50" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="G50" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="H50" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="I50" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
@@ -4345,28 +4342,28 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C51" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="D51" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="E51" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="F51" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="G51" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="H51" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="I51" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -4374,28 +4371,28 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C52" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="D52" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="E52" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="F52" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="G52" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="H52" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="I52" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -4403,28 +4400,28 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C53" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D53" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E53" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="F53" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="G53" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="H53" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="I53" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
@@ -4432,28 +4429,28 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C54" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D54" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E54" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="F54" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="G54" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="H54" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="I54" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -4461,28 +4458,28 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C55" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D55" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E55" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="F55" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="G55" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="H55" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="I55" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -4490,28 +4487,28 @@
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C56" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D56" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E56" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="F56" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="G56" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="H56" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="I56" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -4519,28 +4516,28 @@
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C57" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D57" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E57" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="F57" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="G57" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="H57" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="I57" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -4585,22 +4582,22 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E2" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="F2" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="G2" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -4608,22 +4605,22 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D3" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="E3" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="F3" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="G3" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -4631,22 +4628,22 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D4" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E4" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="F4" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="G4" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -4654,22 +4651,22 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D5" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="E5" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="F5" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="G5" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -4677,22 +4674,22 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D6" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E6" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="F6" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="G6" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -4700,22 +4697,22 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D7" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E7" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="F7" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="G7" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -4723,22 +4720,22 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D8" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E8" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="F8" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="G8" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -4746,22 +4743,22 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D9" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E9" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="F9" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="G9" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -4769,22 +4766,22 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D10" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E10" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="F10" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="G10" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -4792,22 +4789,22 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="E11" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="F11" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="G11" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -4815,22 +4812,22 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="D12" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E12" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="F12" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="G12" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -4838,22 +4835,22 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C13" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D13" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="E13" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="F13" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="G13" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -4861,22 +4858,22 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C14" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D14" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="E14" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="F14" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="G14" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -4884,22 +4881,22 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C15" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D15" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="E15" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="F15" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="G15" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -4907,22 +4904,22 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C16" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D16" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E16" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="F16" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="G16" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -4930,22 +4927,22 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C17" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="D17" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="E17" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="F17" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="G17" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -4953,22 +4950,22 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C18" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="D18" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E18" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="F18" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="G18" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -4976,22 +4973,22 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C19" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D19" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="E19" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="F19" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="G19" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -4999,22 +4996,22 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C20" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D20" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="E20" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="F20" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="G20" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -5022,22 +5019,22 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C21" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D21" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E21" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="F21" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="G21" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -5045,22 +5042,22 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C22" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D22" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E22" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="F22" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="G22" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -5068,22 +5065,22 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C23" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D23" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E23" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="F23" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="G23" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -5091,22 +5088,22 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C24" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D24" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E24" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="F24" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="G24" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -5114,22 +5111,22 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C25" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D25" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E25" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="F25" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="G25" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -5137,22 +5134,22 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="C26" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D26" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E26" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="F26" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="G26" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -5160,22 +5157,22 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C27" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D27" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E27" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="F27" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="G27" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -5183,22 +5180,22 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C28" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D28" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E28" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="F28" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="G28" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -5206,22 +5203,22 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="C29" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D29" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E29" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="F29" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="G29" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -5229,22 +5226,22 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="C30" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D30" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="E30" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="F30" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="G30" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -5252,22 +5249,22 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="C31" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D31" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E31" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="F31" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="G31" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -5275,22 +5272,22 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="C32" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D32" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E32" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="F32" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="G32" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -5298,22 +5295,22 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="C33" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D33" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E33" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="F33" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="G33" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -5321,22 +5318,22 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="C34" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D34" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E34" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="F34" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="G34" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -5344,22 +5341,22 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="C35" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D35" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E35" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="F35" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="G35" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -5367,22 +5364,22 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="C36" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D36" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E36" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="F36" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="G36" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>